<commit_message>
fix: pequenas alteracoes de design
</commit_message>
<xml_diff>
--- a/desafio-xbox.xlsx
+++ b/desafio-xbox.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carol\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f93d456693b9d57a/Documentos/Estudos/Excel/desafio-xbox/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{257D14F4-A439-4562-BB04-07F96EDB08D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{257D14F4-A439-4562-BB04-07F96EDB08D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{903C410B-E0CA-432E-8CAC-13040A8535BF}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{28DD5B76-0634-4F87-BE60-8BFA7EF2E23B}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="3" xr2:uid="{28DD5B76-0634-4F87-BE60-8BFA7EF2E23B}"/>
   </bookViews>
   <sheets>
-    <sheet name="A̳ssets" sheetId="1" r:id="rId1"/>
-    <sheet name="B̳ases" sheetId="2" r:id="rId2"/>
-    <sheet name="C̳álculos" sheetId="3" r:id="rId3"/>
+    <sheet name="A̳ssets" sheetId="1" state="hidden" r:id="rId1"/>
+    <sheet name="B̳ases" sheetId="2" state="hidden" r:id="rId2"/>
+    <sheet name="C̳álculos" sheetId="3" state="hidden" r:id="rId3"/>
     <sheet name="D̳ashboard" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
@@ -24,7 +24,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
@@ -1046,7 +1046,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="&quot;R$&quot;\ #,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -1177,7 +1177,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1203,9 +1203,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
@@ -3105,8 +3103,8 @@
       <xdr:row>4</xdr:row>
       <xdr:rowOff>202403</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="4" name="Subscription Type">
@@ -3129,7 +3127,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -3427,6 +3425,7 @@
                 </a:solidFill>
                 <a:latin typeface="Aptos Narrow"/>
               </a:rPr>
+              <a:pPr algn="ctr"/>
               <a:t>R$ 0,00</a:t>
             </a:fld>
             <a:endParaRPr lang="pt-BR" sz="3600">
@@ -3681,6 +3680,7 @@
                   </a:solidFill>
                   <a:latin typeface="Aptos Narrow"/>
                 </a:rPr>
+                <a:pPr algn="ctr"/>
                 <a:t>R$ 20,00</a:t>
               </a:fld>
               <a:endParaRPr lang="pt-BR" sz="8800">
@@ -4121,6 +4121,7 @@
                 </a:solidFill>
                 <a:latin typeface="Aptos Narrow"/>
               </a:rPr>
+              <a:pPr algn="ctr"/>
               <a:t>1</a:t>
             </a:fld>
             <a:endParaRPr lang="en-US" sz="3600" b="0" i="0" u="none" strike="noStrike">
@@ -4357,6 +4358,7 @@
                 </a:solidFill>
                 <a:latin typeface="Aptos Narrow"/>
               </a:rPr>
+              <a:pPr algn="ctr"/>
               <a:t>R$ 10,00</a:t>
             </a:fld>
             <a:endParaRPr lang="en-US" sz="3600" b="0" i="0" u="none" strike="noStrike">
@@ -4373,16 +4375,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>357188</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>178594</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>59531</xdr:rowOff>
+      <xdr:rowOff>107156</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>202406</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>23812</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>157162</xdr:rowOff>
+      <xdr:rowOff>154781</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:tsle="http://schemas.microsoft.com/office/drawing/2012/timeslicer" Requires="tsle">
@@ -4418,8 +4420,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="4631532" y="1297781"/>
-              <a:ext cx="5143499" cy="1264444"/>
+              <a:off x="2631282" y="1345406"/>
+              <a:ext cx="5143499" cy="1214438"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -9523,673 +9525,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F6B7CC1D-7751-47E1-92C9-F61E2A5AAB63}" name="Tabela dinâmica4" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="5" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
-  <location ref="C47:D49" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="13">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="281">
-        <item x="87"/>
-        <item x="61"/>
-        <item x="206"/>
-        <item x="275"/>
-        <item x="112"/>
-        <item x="228"/>
-        <item x="35"/>
-        <item x="253"/>
-        <item x="136"/>
-        <item x="3"/>
-        <item x="161"/>
-        <item x="185"/>
-        <item x="7"/>
-        <item x="88"/>
-        <item x="16"/>
-        <item x="186"/>
-        <item x="162"/>
-        <item x="276"/>
-        <item x="36"/>
-        <item x="254"/>
-        <item x="207"/>
-        <item x="137"/>
-        <item x="62"/>
-        <item x="9"/>
-        <item x="113"/>
-        <item x="229"/>
-        <item x="163"/>
-        <item x="15"/>
-        <item x="6"/>
-        <item x="63"/>
-        <item x="37"/>
-        <item x="230"/>
-        <item x="255"/>
-        <item x="277"/>
-        <item x="138"/>
-        <item x="89"/>
-        <item x="114"/>
-        <item x="17"/>
-        <item x="187"/>
-        <item x="90"/>
-        <item x="139"/>
-        <item x="18"/>
-        <item x="38"/>
-        <item x="64"/>
-        <item x="231"/>
-        <item x="208"/>
-        <item x="256"/>
-        <item x="278"/>
-        <item x="13"/>
-        <item x="115"/>
-        <item x="164"/>
-        <item x="91"/>
-        <item x="188"/>
-        <item x="19"/>
-        <item x="209"/>
-        <item x="116"/>
-        <item x="257"/>
-        <item x="279"/>
-        <item x="140"/>
-        <item x="65"/>
-        <item x="39"/>
-        <item x="92"/>
-        <item x="210"/>
-        <item x="141"/>
-        <item x="232"/>
-        <item x="258"/>
-        <item x="40"/>
-        <item x="66"/>
-        <item x="117"/>
-        <item x="5"/>
-        <item x="165"/>
-        <item x="14"/>
-        <item x="67"/>
-        <item x="211"/>
-        <item x="189"/>
-        <item x="259"/>
-        <item x="20"/>
-        <item x="93"/>
-        <item x="233"/>
-        <item x="41"/>
-        <item x="142"/>
-        <item x="166"/>
-        <item x="143"/>
-        <item x="94"/>
-        <item x="212"/>
-        <item x="167"/>
-        <item x="68"/>
-        <item x="42"/>
-        <item x="234"/>
-        <item x="118"/>
-        <item x="21"/>
-        <item x="260"/>
-        <item x="144"/>
-        <item x="190"/>
-        <item x="213"/>
-        <item x="168"/>
-        <item x="43"/>
-        <item x="235"/>
-        <item x="119"/>
-        <item x="95"/>
-        <item x="22"/>
-        <item x="69"/>
-        <item x="145"/>
-        <item x="191"/>
-        <item x="169"/>
-        <item x="120"/>
-        <item x="261"/>
-        <item x="96"/>
-        <item x="236"/>
-        <item x="0"/>
-        <item x="23"/>
-        <item x="44"/>
-        <item x="70"/>
-        <item x="71"/>
-        <item x="97"/>
-        <item x="170"/>
-        <item x="262"/>
-        <item x="237"/>
-        <item x="146"/>
-        <item x="45"/>
-        <item x="24"/>
-        <item x="121"/>
-        <item x="12"/>
-        <item x="2"/>
-        <item x="192"/>
-        <item x="72"/>
-        <item x="263"/>
-        <item x="171"/>
-        <item x="238"/>
-        <item x="46"/>
-        <item x="98"/>
-        <item x="214"/>
-        <item x="147"/>
-        <item x="193"/>
-        <item x="264"/>
-        <item x="99"/>
-        <item x="172"/>
-        <item x="47"/>
-        <item x="122"/>
-        <item x="11"/>
-        <item x="239"/>
-        <item x="148"/>
-        <item x="215"/>
-        <item x="1"/>
-        <item x="25"/>
-        <item x="73"/>
-        <item x="123"/>
-        <item x="216"/>
-        <item x="265"/>
-        <item x="149"/>
-        <item x="240"/>
-        <item x="194"/>
-        <item x="26"/>
-        <item x="48"/>
-        <item x="173"/>
-        <item x="100"/>
-        <item x="74"/>
-        <item x="195"/>
-        <item x="174"/>
-        <item x="124"/>
-        <item x="241"/>
-        <item x="266"/>
-        <item x="49"/>
-        <item x="101"/>
-        <item x="150"/>
-        <item x="217"/>
-        <item x="75"/>
-        <item x="27"/>
-        <item x="151"/>
-        <item x="102"/>
-        <item x="218"/>
-        <item x="242"/>
-        <item x="267"/>
-        <item x="125"/>
-        <item x="50"/>
-        <item x="28"/>
-        <item x="76"/>
-        <item x="196"/>
-        <item x="175"/>
-        <item x="4"/>
-        <item x="126"/>
-        <item x="219"/>
-        <item x="268"/>
-        <item x="77"/>
-        <item x="51"/>
-        <item x="152"/>
-        <item x="243"/>
-        <item x="127"/>
-        <item x="103"/>
-        <item x="244"/>
-        <item x="29"/>
-        <item x="197"/>
-        <item x="176"/>
-        <item x="78"/>
-        <item x="269"/>
-        <item x="52"/>
-        <item x="153"/>
-        <item x="10"/>
-        <item x="79"/>
-        <item x="104"/>
-        <item x="30"/>
-        <item x="177"/>
-        <item x="220"/>
-        <item x="245"/>
-        <item x="270"/>
-        <item x="128"/>
-        <item x="8"/>
-        <item x="154"/>
-        <item x="198"/>
-        <item x="53"/>
-        <item x="31"/>
-        <item x="271"/>
-        <item x="246"/>
-        <item x="105"/>
-        <item x="178"/>
-        <item x="221"/>
-        <item x="80"/>
-        <item x="129"/>
-        <item x="155"/>
-        <item x="54"/>
-        <item x="199"/>
-        <item x="247"/>
-        <item x="55"/>
-        <item x="106"/>
-        <item x="179"/>
-        <item x="81"/>
-        <item x="156"/>
-        <item x="222"/>
-        <item x="200"/>
-        <item x="130"/>
-        <item x="248"/>
-        <item x="56"/>
-        <item x="223"/>
-        <item x="157"/>
-        <item x="131"/>
-        <item x="180"/>
-        <item x="201"/>
-        <item x="82"/>
-        <item x="107"/>
-        <item x="32"/>
-        <item x="158"/>
-        <item x="132"/>
-        <item x="202"/>
-        <item x="83"/>
-        <item x="181"/>
-        <item x="224"/>
-        <item x="249"/>
-        <item x="57"/>
-        <item x="108"/>
-        <item x="203"/>
-        <item x="133"/>
-        <item x="225"/>
-        <item x="109"/>
-        <item x="272"/>
-        <item x="182"/>
-        <item x="84"/>
-        <item x="250"/>
-        <item x="58"/>
-        <item x="110"/>
-        <item x="59"/>
-        <item x="183"/>
-        <item x="226"/>
-        <item x="85"/>
-        <item x="273"/>
-        <item x="159"/>
-        <item x="33"/>
-        <item x="204"/>
-        <item x="251"/>
-        <item x="134"/>
-        <item x="205"/>
-        <item x="60"/>
-        <item x="184"/>
-        <item x="160"/>
-        <item x="274"/>
-        <item x="227"/>
-        <item x="135"/>
-        <item x="86"/>
-        <item x="34"/>
-        <item x="252"/>
-        <item x="111"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="4">
-        <item x="1"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField numFmtId="14" showAll="0">
-      <items count="295">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="4"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="13"/>
-        <item x="14"/>
-        <item x="15"/>
-        <item x="16"/>
-        <item x="17"/>
-        <item x="18"/>
-        <item x="19"/>
-        <item x="20"/>
-        <item x="21"/>
-        <item x="22"/>
-        <item x="23"/>
-        <item x="24"/>
-        <item x="25"/>
-        <item x="26"/>
-        <item x="27"/>
-        <item x="28"/>
-        <item x="29"/>
-        <item x="30"/>
-        <item x="31"/>
-        <item x="32"/>
-        <item x="33"/>
-        <item x="34"/>
-        <item x="35"/>
-        <item x="36"/>
-        <item x="37"/>
-        <item x="38"/>
-        <item x="39"/>
-        <item x="40"/>
-        <item x="41"/>
-        <item x="42"/>
-        <item x="43"/>
-        <item x="44"/>
-        <item x="45"/>
-        <item x="46"/>
-        <item x="47"/>
-        <item x="48"/>
-        <item x="49"/>
-        <item x="50"/>
-        <item x="51"/>
-        <item x="52"/>
-        <item x="53"/>
-        <item x="54"/>
-        <item x="55"/>
-        <item x="56"/>
-        <item x="57"/>
-        <item x="58"/>
-        <item x="59"/>
-        <item x="60"/>
-        <item x="61"/>
-        <item x="62"/>
-        <item x="63"/>
-        <item x="64"/>
-        <item x="65"/>
-        <item x="66"/>
-        <item x="67"/>
-        <item x="68"/>
-        <item x="69"/>
-        <item x="70"/>
-        <item x="71"/>
-        <item x="72"/>
-        <item x="73"/>
-        <item x="74"/>
-        <item x="75"/>
-        <item x="76"/>
-        <item x="77"/>
-        <item x="78"/>
-        <item x="79"/>
-        <item x="80"/>
-        <item x="81"/>
-        <item x="82"/>
-        <item x="83"/>
-        <item x="84"/>
-        <item x="85"/>
-        <item x="86"/>
-        <item x="87"/>
-        <item x="88"/>
-        <item x="89"/>
-        <item x="90"/>
-        <item x="91"/>
-        <item x="92"/>
-        <item x="93"/>
-        <item x="94"/>
-        <item x="95"/>
-        <item x="96"/>
-        <item x="97"/>
-        <item x="98"/>
-        <item x="99"/>
-        <item x="100"/>
-        <item x="101"/>
-        <item x="102"/>
-        <item x="103"/>
-        <item x="104"/>
-        <item x="105"/>
-        <item x="106"/>
-        <item x="107"/>
-        <item x="108"/>
-        <item x="109"/>
-        <item x="110"/>
-        <item x="111"/>
-        <item x="112"/>
-        <item x="113"/>
-        <item x="114"/>
-        <item x="115"/>
-        <item x="116"/>
-        <item x="117"/>
-        <item x="118"/>
-        <item x="119"/>
-        <item x="120"/>
-        <item x="121"/>
-        <item x="122"/>
-        <item x="123"/>
-        <item x="124"/>
-        <item x="125"/>
-        <item x="126"/>
-        <item x="127"/>
-        <item x="128"/>
-        <item x="129"/>
-        <item x="130"/>
-        <item x="131"/>
-        <item x="132"/>
-        <item x="133"/>
-        <item x="134"/>
-        <item x="135"/>
-        <item x="136"/>
-        <item x="137"/>
-        <item x="138"/>
-        <item x="139"/>
-        <item x="140"/>
-        <item x="141"/>
-        <item x="142"/>
-        <item x="143"/>
-        <item x="144"/>
-        <item x="145"/>
-        <item x="146"/>
-        <item x="147"/>
-        <item x="148"/>
-        <item x="149"/>
-        <item x="150"/>
-        <item x="151"/>
-        <item x="152"/>
-        <item x="153"/>
-        <item x="154"/>
-        <item x="155"/>
-        <item x="156"/>
-        <item x="157"/>
-        <item x="158"/>
-        <item x="159"/>
-        <item x="160"/>
-        <item x="161"/>
-        <item x="162"/>
-        <item x="163"/>
-        <item x="164"/>
-        <item x="165"/>
-        <item x="166"/>
-        <item x="167"/>
-        <item x="168"/>
-        <item x="169"/>
-        <item x="170"/>
-        <item x="171"/>
-        <item x="172"/>
-        <item x="173"/>
-        <item x="174"/>
-        <item x="175"/>
-        <item x="176"/>
-        <item x="177"/>
-        <item x="178"/>
-        <item x="179"/>
-        <item x="180"/>
-        <item x="181"/>
-        <item x="182"/>
-        <item x="183"/>
-        <item x="184"/>
-        <item x="185"/>
-        <item x="186"/>
-        <item x="187"/>
-        <item x="188"/>
-        <item x="189"/>
-        <item x="190"/>
-        <item x="191"/>
-        <item x="192"/>
-        <item x="193"/>
-        <item x="194"/>
-        <item x="195"/>
-        <item x="196"/>
-        <item x="197"/>
-        <item x="198"/>
-        <item x="199"/>
-        <item x="200"/>
-        <item x="201"/>
-        <item x="202"/>
-        <item x="203"/>
-        <item x="204"/>
-        <item x="205"/>
-        <item x="206"/>
-        <item x="207"/>
-        <item x="208"/>
-        <item x="209"/>
-        <item x="210"/>
-        <item x="211"/>
-        <item x="212"/>
-        <item x="213"/>
-        <item x="214"/>
-        <item x="215"/>
-        <item x="216"/>
-        <item x="217"/>
-        <item x="218"/>
-        <item x="219"/>
-        <item x="220"/>
-        <item x="221"/>
-        <item x="222"/>
-        <item x="223"/>
-        <item x="224"/>
-        <item x="225"/>
-        <item x="226"/>
-        <item x="227"/>
-        <item x="228"/>
-        <item x="229"/>
-        <item x="230"/>
-        <item x="231"/>
-        <item x="232"/>
-        <item x="233"/>
-        <item x="234"/>
-        <item x="235"/>
-        <item x="236"/>
-        <item x="237"/>
-        <item x="238"/>
-        <item x="239"/>
-        <item x="240"/>
-        <item x="241"/>
-        <item x="242"/>
-        <item x="243"/>
-        <item x="244"/>
-        <item x="245"/>
-        <item x="246"/>
-        <item x="247"/>
-        <item x="248"/>
-        <item x="249"/>
-        <item x="250"/>
-        <item x="251"/>
-        <item x="252"/>
-        <item x="253"/>
-        <item x="254"/>
-        <item x="255"/>
-        <item x="256"/>
-        <item x="257"/>
-        <item x="258"/>
-        <item x="259"/>
-        <item x="260"/>
-        <item x="261"/>
-        <item x="262"/>
-        <item x="263"/>
-        <item x="264"/>
-        <item x="265"/>
-        <item x="266"/>
-        <item x="267"/>
-        <item x="268"/>
-        <item x="269"/>
-        <item x="270"/>
-        <item x="271"/>
-        <item x="272"/>
-        <item x="273"/>
-        <item x="274"/>
-        <item x="275"/>
-        <item x="276"/>
-        <item x="277"/>
-        <item x="278"/>
-        <item x="279"/>
-        <item x="280"/>
-        <item x="281"/>
-        <item x="282"/>
-        <item x="283"/>
-        <item x="284"/>
-        <item x="285"/>
-        <item x="286"/>
-        <item x="287"/>
-        <item x="288"/>
-        <item x="289"/>
-        <item x="290"/>
-        <item x="291"/>
-        <item x="292"/>
-        <item x="293"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField numFmtId="44" showAll="0"/>
-    <pivotField showAll="0">
-      <items count="4">
-        <item h="1" x="1"/>
-        <item h="1" x="0"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="44" showAll="0"/>
-    <pivotField dataField="1" numFmtId="44" showAll="0"/>
-    <pivotField numFmtId="44" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="2"/>
-  </rowFields>
-  <rowItems count="2">
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Soma de Coupon Value" fld="11" baseField="0" baseItem="0" numFmtId="44"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <filters count="1">
-    <filter fld="3" type="dateBetween" evalOrder="-1" id="13" name="Start Date">
-      <autoFilter ref="A1">
-        <filterColumn colId="0">
-          <customFilters and="1">
-            <customFilter operator="greaterThanOrEqual" val="45323"/>
-            <customFilter operator="lessThanOrEqual" val="45351"/>
-          </customFilters>
-        </filterColumn>
-      </autoFilter>
-      <extLst>
-        <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{0605FD5F-26C8-4aeb-8148-2DB25E43C511}">
-          <x15:pivotFilter useWholeDay="1"/>
-        </ext>
-      </extLst>
-    </filter>
-  </filters>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9D73167F-55CC-4576-925F-446277351334}" name="Tabela dinâmica3" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="5" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9D73167F-55CC-4576-925F-446277351334}" name="Tabela dinâmica3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="5" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
   <location ref="C40:D42" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="13">
     <pivotField dataField="1" showAll="0"/>
@@ -10854,8 +10190,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{711D6553-0954-4A49-A55D-3666F70C3251}" name="Tabela dinâmica2" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="5" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{711D6553-0954-4A49-A55D-3666F70C3251}" name="Tabela dinâmica2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="5" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
   <location ref="C33:D35" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="13">
     <pivotField showAll="0"/>
@@ -11520,8 +10856,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{DB98B642-8467-4890-8652-830405390682}" name="tbld_easeasonpass_annual" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="5" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{DB98B642-8467-4890-8652-830405390682}" name="tbld_easeasonpass_annual" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="5" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
   <location ref="C25:D27" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="13">
     <pivotField showAll="0"/>
@@ -12186,8 +11522,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7DC90952-D2EE-41D1-A780-B278666670CA}" name="tlbd_annual_total" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="5" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7DC90952-D2EE-41D1-A780-B278666670CA}" name="tlbd_annual_total" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="5" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
   <location ref="C14:D16" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="13">
     <pivotField showAll="0"/>
@@ -12859,6 +12195,672 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F6B7CC1D-7751-47E1-92C9-F61E2A5AAB63}" name="Tabela dinâmica4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="5" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
+  <location ref="C47:D49" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="13">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="281">
+        <item x="87"/>
+        <item x="61"/>
+        <item x="206"/>
+        <item x="275"/>
+        <item x="112"/>
+        <item x="228"/>
+        <item x="35"/>
+        <item x="253"/>
+        <item x="136"/>
+        <item x="3"/>
+        <item x="161"/>
+        <item x="185"/>
+        <item x="7"/>
+        <item x="88"/>
+        <item x="16"/>
+        <item x="186"/>
+        <item x="162"/>
+        <item x="276"/>
+        <item x="36"/>
+        <item x="254"/>
+        <item x="207"/>
+        <item x="137"/>
+        <item x="62"/>
+        <item x="9"/>
+        <item x="113"/>
+        <item x="229"/>
+        <item x="163"/>
+        <item x="15"/>
+        <item x="6"/>
+        <item x="63"/>
+        <item x="37"/>
+        <item x="230"/>
+        <item x="255"/>
+        <item x="277"/>
+        <item x="138"/>
+        <item x="89"/>
+        <item x="114"/>
+        <item x="17"/>
+        <item x="187"/>
+        <item x="90"/>
+        <item x="139"/>
+        <item x="18"/>
+        <item x="38"/>
+        <item x="64"/>
+        <item x="231"/>
+        <item x="208"/>
+        <item x="256"/>
+        <item x="278"/>
+        <item x="13"/>
+        <item x="115"/>
+        <item x="164"/>
+        <item x="91"/>
+        <item x="188"/>
+        <item x="19"/>
+        <item x="209"/>
+        <item x="116"/>
+        <item x="257"/>
+        <item x="279"/>
+        <item x="140"/>
+        <item x="65"/>
+        <item x="39"/>
+        <item x="92"/>
+        <item x="210"/>
+        <item x="141"/>
+        <item x="232"/>
+        <item x="258"/>
+        <item x="40"/>
+        <item x="66"/>
+        <item x="117"/>
+        <item x="5"/>
+        <item x="165"/>
+        <item x="14"/>
+        <item x="67"/>
+        <item x="211"/>
+        <item x="189"/>
+        <item x="259"/>
+        <item x="20"/>
+        <item x="93"/>
+        <item x="233"/>
+        <item x="41"/>
+        <item x="142"/>
+        <item x="166"/>
+        <item x="143"/>
+        <item x="94"/>
+        <item x="212"/>
+        <item x="167"/>
+        <item x="68"/>
+        <item x="42"/>
+        <item x="234"/>
+        <item x="118"/>
+        <item x="21"/>
+        <item x="260"/>
+        <item x="144"/>
+        <item x="190"/>
+        <item x="213"/>
+        <item x="168"/>
+        <item x="43"/>
+        <item x="235"/>
+        <item x="119"/>
+        <item x="95"/>
+        <item x="22"/>
+        <item x="69"/>
+        <item x="145"/>
+        <item x="191"/>
+        <item x="169"/>
+        <item x="120"/>
+        <item x="261"/>
+        <item x="96"/>
+        <item x="236"/>
+        <item x="0"/>
+        <item x="23"/>
+        <item x="44"/>
+        <item x="70"/>
+        <item x="71"/>
+        <item x="97"/>
+        <item x="170"/>
+        <item x="262"/>
+        <item x="237"/>
+        <item x="146"/>
+        <item x="45"/>
+        <item x="24"/>
+        <item x="121"/>
+        <item x="12"/>
+        <item x="2"/>
+        <item x="192"/>
+        <item x="72"/>
+        <item x="263"/>
+        <item x="171"/>
+        <item x="238"/>
+        <item x="46"/>
+        <item x="98"/>
+        <item x="214"/>
+        <item x="147"/>
+        <item x="193"/>
+        <item x="264"/>
+        <item x="99"/>
+        <item x="172"/>
+        <item x="47"/>
+        <item x="122"/>
+        <item x="11"/>
+        <item x="239"/>
+        <item x="148"/>
+        <item x="215"/>
+        <item x="1"/>
+        <item x="25"/>
+        <item x="73"/>
+        <item x="123"/>
+        <item x="216"/>
+        <item x="265"/>
+        <item x="149"/>
+        <item x="240"/>
+        <item x="194"/>
+        <item x="26"/>
+        <item x="48"/>
+        <item x="173"/>
+        <item x="100"/>
+        <item x="74"/>
+        <item x="195"/>
+        <item x="174"/>
+        <item x="124"/>
+        <item x="241"/>
+        <item x="266"/>
+        <item x="49"/>
+        <item x="101"/>
+        <item x="150"/>
+        <item x="217"/>
+        <item x="75"/>
+        <item x="27"/>
+        <item x="151"/>
+        <item x="102"/>
+        <item x="218"/>
+        <item x="242"/>
+        <item x="267"/>
+        <item x="125"/>
+        <item x="50"/>
+        <item x="28"/>
+        <item x="76"/>
+        <item x="196"/>
+        <item x="175"/>
+        <item x="4"/>
+        <item x="126"/>
+        <item x="219"/>
+        <item x="268"/>
+        <item x="77"/>
+        <item x="51"/>
+        <item x="152"/>
+        <item x="243"/>
+        <item x="127"/>
+        <item x="103"/>
+        <item x="244"/>
+        <item x="29"/>
+        <item x="197"/>
+        <item x="176"/>
+        <item x="78"/>
+        <item x="269"/>
+        <item x="52"/>
+        <item x="153"/>
+        <item x="10"/>
+        <item x="79"/>
+        <item x="104"/>
+        <item x="30"/>
+        <item x="177"/>
+        <item x="220"/>
+        <item x="245"/>
+        <item x="270"/>
+        <item x="128"/>
+        <item x="8"/>
+        <item x="154"/>
+        <item x="198"/>
+        <item x="53"/>
+        <item x="31"/>
+        <item x="271"/>
+        <item x="246"/>
+        <item x="105"/>
+        <item x="178"/>
+        <item x="221"/>
+        <item x="80"/>
+        <item x="129"/>
+        <item x="155"/>
+        <item x="54"/>
+        <item x="199"/>
+        <item x="247"/>
+        <item x="55"/>
+        <item x="106"/>
+        <item x="179"/>
+        <item x="81"/>
+        <item x="156"/>
+        <item x="222"/>
+        <item x="200"/>
+        <item x="130"/>
+        <item x="248"/>
+        <item x="56"/>
+        <item x="223"/>
+        <item x="157"/>
+        <item x="131"/>
+        <item x="180"/>
+        <item x="201"/>
+        <item x="82"/>
+        <item x="107"/>
+        <item x="32"/>
+        <item x="158"/>
+        <item x="132"/>
+        <item x="202"/>
+        <item x="83"/>
+        <item x="181"/>
+        <item x="224"/>
+        <item x="249"/>
+        <item x="57"/>
+        <item x="108"/>
+        <item x="203"/>
+        <item x="133"/>
+        <item x="225"/>
+        <item x="109"/>
+        <item x="272"/>
+        <item x="182"/>
+        <item x="84"/>
+        <item x="250"/>
+        <item x="58"/>
+        <item x="110"/>
+        <item x="59"/>
+        <item x="183"/>
+        <item x="226"/>
+        <item x="85"/>
+        <item x="273"/>
+        <item x="159"/>
+        <item x="33"/>
+        <item x="204"/>
+        <item x="251"/>
+        <item x="134"/>
+        <item x="205"/>
+        <item x="60"/>
+        <item x="184"/>
+        <item x="160"/>
+        <item x="274"/>
+        <item x="227"/>
+        <item x="135"/>
+        <item x="86"/>
+        <item x="34"/>
+        <item x="252"/>
+        <item x="111"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="14" showAll="0">
+      <items count="295">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="4"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="19"/>
+        <item x="20"/>
+        <item x="21"/>
+        <item x="22"/>
+        <item x="23"/>
+        <item x="24"/>
+        <item x="25"/>
+        <item x="26"/>
+        <item x="27"/>
+        <item x="28"/>
+        <item x="29"/>
+        <item x="30"/>
+        <item x="31"/>
+        <item x="32"/>
+        <item x="33"/>
+        <item x="34"/>
+        <item x="35"/>
+        <item x="36"/>
+        <item x="37"/>
+        <item x="38"/>
+        <item x="39"/>
+        <item x="40"/>
+        <item x="41"/>
+        <item x="42"/>
+        <item x="43"/>
+        <item x="44"/>
+        <item x="45"/>
+        <item x="46"/>
+        <item x="47"/>
+        <item x="48"/>
+        <item x="49"/>
+        <item x="50"/>
+        <item x="51"/>
+        <item x="52"/>
+        <item x="53"/>
+        <item x="54"/>
+        <item x="55"/>
+        <item x="56"/>
+        <item x="57"/>
+        <item x="58"/>
+        <item x="59"/>
+        <item x="60"/>
+        <item x="61"/>
+        <item x="62"/>
+        <item x="63"/>
+        <item x="64"/>
+        <item x="65"/>
+        <item x="66"/>
+        <item x="67"/>
+        <item x="68"/>
+        <item x="69"/>
+        <item x="70"/>
+        <item x="71"/>
+        <item x="72"/>
+        <item x="73"/>
+        <item x="74"/>
+        <item x="75"/>
+        <item x="76"/>
+        <item x="77"/>
+        <item x="78"/>
+        <item x="79"/>
+        <item x="80"/>
+        <item x="81"/>
+        <item x="82"/>
+        <item x="83"/>
+        <item x="84"/>
+        <item x="85"/>
+        <item x="86"/>
+        <item x="87"/>
+        <item x="88"/>
+        <item x="89"/>
+        <item x="90"/>
+        <item x="91"/>
+        <item x="92"/>
+        <item x="93"/>
+        <item x="94"/>
+        <item x="95"/>
+        <item x="96"/>
+        <item x="97"/>
+        <item x="98"/>
+        <item x="99"/>
+        <item x="100"/>
+        <item x="101"/>
+        <item x="102"/>
+        <item x="103"/>
+        <item x="104"/>
+        <item x="105"/>
+        <item x="106"/>
+        <item x="107"/>
+        <item x="108"/>
+        <item x="109"/>
+        <item x="110"/>
+        <item x="111"/>
+        <item x="112"/>
+        <item x="113"/>
+        <item x="114"/>
+        <item x="115"/>
+        <item x="116"/>
+        <item x="117"/>
+        <item x="118"/>
+        <item x="119"/>
+        <item x="120"/>
+        <item x="121"/>
+        <item x="122"/>
+        <item x="123"/>
+        <item x="124"/>
+        <item x="125"/>
+        <item x="126"/>
+        <item x="127"/>
+        <item x="128"/>
+        <item x="129"/>
+        <item x="130"/>
+        <item x="131"/>
+        <item x="132"/>
+        <item x="133"/>
+        <item x="134"/>
+        <item x="135"/>
+        <item x="136"/>
+        <item x="137"/>
+        <item x="138"/>
+        <item x="139"/>
+        <item x="140"/>
+        <item x="141"/>
+        <item x="142"/>
+        <item x="143"/>
+        <item x="144"/>
+        <item x="145"/>
+        <item x="146"/>
+        <item x="147"/>
+        <item x="148"/>
+        <item x="149"/>
+        <item x="150"/>
+        <item x="151"/>
+        <item x="152"/>
+        <item x="153"/>
+        <item x="154"/>
+        <item x="155"/>
+        <item x="156"/>
+        <item x="157"/>
+        <item x="158"/>
+        <item x="159"/>
+        <item x="160"/>
+        <item x="161"/>
+        <item x="162"/>
+        <item x="163"/>
+        <item x="164"/>
+        <item x="165"/>
+        <item x="166"/>
+        <item x="167"/>
+        <item x="168"/>
+        <item x="169"/>
+        <item x="170"/>
+        <item x="171"/>
+        <item x="172"/>
+        <item x="173"/>
+        <item x="174"/>
+        <item x="175"/>
+        <item x="176"/>
+        <item x="177"/>
+        <item x="178"/>
+        <item x="179"/>
+        <item x="180"/>
+        <item x="181"/>
+        <item x="182"/>
+        <item x="183"/>
+        <item x="184"/>
+        <item x="185"/>
+        <item x="186"/>
+        <item x="187"/>
+        <item x="188"/>
+        <item x="189"/>
+        <item x="190"/>
+        <item x="191"/>
+        <item x="192"/>
+        <item x="193"/>
+        <item x="194"/>
+        <item x="195"/>
+        <item x="196"/>
+        <item x="197"/>
+        <item x="198"/>
+        <item x="199"/>
+        <item x="200"/>
+        <item x="201"/>
+        <item x="202"/>
+        <item x="203"/>
+        <item x="204"/>
+        <item x="205"/>
+        <item x="206"/>
+        <item x="207"/>
+        <item x="208"/>
+        <item x="209"/>
+        <item x="210"/>
+        <item x="211"/>
+        <item x="212"/>
+        <item x="213"/>
+        <item x="214"/>
+        <item x="215"/>
+        <item x="216"/>
+        <item x="217"/>
+        <item x="218"/>
+        <item x="219"/>
+        <item x="220"/>
+        <item x="221"/>
+        <item x="222"/>
+        <item x="223"/>
+        <item x="224"/>
+        <item x="225"/>
+        <item x="226"/>
+        <item x="227"/>
+        <item x="228"/>
+        <item x="229"/>
+        <item x="230"/>
+        <item x="231"/>
+        <item x="232"/>
+        <item x="233"/>
+        <item x="234"/>
+        <item x="235"/>
+        <item x="236"/>
+        <item x="237"/>
+        <item x="238"/>
+        <item x="239"/>
+        <item x="240"/>
+        <item x="241"/>
+        <item x="242"/>
+        <item x="243"/>
+        <item x="244"/>
+        <item x="245"/>
+        <item x="246"/>
+        <item x="247"/>
+        <item x="248"/>
+        <item x="249"/>
+        <item x="250"/>
+        <item x="251"/>
+        <item x="252"/>
+        <item x="253"/>
+        <item x="254"/>
+        <item x="255"/>
+        <item x="256"/>
+        <item x="257"/>
+        <item x="258"/>
+        <item x="259"/>
+        <item x="260"/>
+        <item x="261"/>
+        <item x="262"/>
+        <item x="263"/>
+        <item x="264"/>
+        <item x="265"/>
+        <item x="266"/>
+        <item x="267"/>
+        <item x="268"/>
+        <item x="269"/>
+        <item x="270"/>
+        <item x="271"/>
+        <item x="272"/>
+        <item x="273"/>
+        <item x="274"/>
+        <item x="275"/>
+        <item x="276"/>
+        <item x="277"/>
+        <item x="278"/>
+        <item x="279"/>
+        <item x="280"/>
+        <item x="281"/>
+        <item x="282"/>
+        <item x="283"/>
+        <item x="284"/>
+        <item x="285"/>
+        <item x="286"/>
+        <item x="287"/>
+        <item x="288"/>
+        <item x="289"/>
+        <item x="290"/>
+        <item x="291"/>
+        <item x="292"/>
+        <item x="293"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="44" showAll="0"/>
+    <pivotField showAll="0">
+      <items count="4">
+        <item h="1" x="1"/>
+        <item h="1" x="0"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="44" showAll="0"/>
+    <pivotField dataField="1" numFmtId="44" showAll="0"/>
+    <pivotField numFmtId="44" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="2">
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Soma de Coupon Value" fld="11" baseField="0" baseItem="0" numFmtId="44"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <filters count="1">
+    <filter fld="3" type="dateBetween" evalOrder="-1" id="13" name="Start Date">
+      <autoFilter ref="A1">
+        <filterColumn colId="0">
+          <customFilters and="1">
+            <customFilter operator="greaterThanOrEqual" val="45323"/>
+            <customFilter operator="lessThanOrEqual" val="45351"/>
+          </customFilters>
+        </filterColumn>
+      </autoFilter>
+      <extLst>
+        <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{0605FD5F-26C8-4aeb-8148-2DB25E43C511}">
+          <x15:pivotFilter useWholeDay="1"/>
+        </ext>
+      </extLst>
+    </filter>
+  </filters>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/slicerCaches/slicerCache1.xml><?xml version="1.0" encoding="utf-8"?>
 <slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="SegmentaçãodeDados_Subscription_Type" xr10:uid="{14A4888F-18E3-4FF3-BFD3-A338BEA35414}" sourceName="Subscription Type">
   <pivotTables>
@@ -13253,7 +13255,7 @@
   <dimension ref="B3:P21"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13426,7 +13428,7 @@
   <dimension ref="A1:M296"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25660,7 +25662,7 @@
       </c>
     </row>
     <row r="24" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D24" s="16">
+      <c r="D24" s="15">
         <f>GETPIVOTDATA("EA Play Season Pass
 Price",$C$25)</f>
         <v>0</v>
@@ -25678,7 +25680,7 @@
       <c r="C26" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="D26" s="15">
+      <c r="D26">
         <v>0</v>
       </c>
     </row>
@@ -25686,7 +25688,7 @@
       <c r="C27" s="13" t="s">
         <v>314</v>
       </c>
-      <c r="D27" s="15">
+      <c r="D27">
         <v>0</v>
       </c>
     </row>
@@ -25696,7 +25698,7 @@
       </c>
     </row>
     <row r="32" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D32" s="16">
+      <c r="D32" s="15">
         <f>GETPIVOTDATA("Minecraft Season Pass Price",$C$33)</f>
         <v>20</v>
       </c>
@@ -25748,7 +25750,7 @@
       <c r="C41" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="D41" s="15">
+      <c r="D41">
         <v>1</v>
       </c>
     </row>
@@ -25756,7 +25758,7 @@
       <c r="C42" s="13" t="s">
         <v>314</v>
       </c>
-      <c r="D42" s="15">
+      <c r="D42">
         <v>1</v>
       </c>
     </row>
@@ -25766,7 +25768,7 @@
       </c>
     </row>
     <row r="46" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D46" s="16">
+      <c r="D46" s="15">
         <f>GETPIVOTDATA("Coupon Value",$C$47)</f>
         <v>10</v>
       </c>
@@ -25803,929 +25805,339 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{210F14EF-C0B7-459D-9E09-3130BA4314A6}">
-  <dimension ref="A1:R300"/>
+  <dimension ref="C1:R300"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="V9" sqref="V9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15" style="17" customWidth="1"/>
+    <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="3.5703125" customWidth="1"/>
     <col min="12" max="12" width="6.5703125" customWidth="1"/>
     <col min="18" max="18" width="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="18" customFormat="1" ht="79.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:18" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C2" s="19" t="s">
+    <row r="1" spans="3:18" s="16" customFormat="1" ht="79.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="3:18" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C2" s="17" t="s">
         <v>316</v>
       </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="19"/>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="19"/>
-      <c r="R2" s="19"/>
-    </row>
-    <row r="3" spans="1:18" ht="75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:18" s="7" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="17"/>
-    </row>
-    <row r="7" spans="1:18" s="7" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="17"/>
-    </row>
-    <row r="8" spans="1:18" s="7" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="17"/>
-    </row>
-    <row r="9" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="17"/>
-    </row>
-    <row r="10" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="17"/>
-    </row>
-    <row r="11" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="17"/>
-    </row>
-    <row r="12" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="17"/>
-    </row>
-    <row r="13" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="17"/>
-    </row>
-    <row r="14" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="17"/>
-    </row>
-    <row r="15" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="17"/>
-    </row>
-    <row r="16" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="17"/>
-    </row>
-    <row r="17" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="17"/>
-    </row>
-    <row r="18" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="17"/>
-    </row>
-    <row r="19" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="17"/>
-    </row>
-    <row r="20" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="17"/>
-    </row>
-    <row r="21" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="17"/>
-    </row>
-    <row r="22" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="17"/>
-    </row>
-    <row r="23" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="17"/>
-    </row>
-    <row r="24" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="17"/>
-    </row>
-    <row r="25" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="17"/>
-    </row>
-    <row r="26" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="17"/>
-    </row>
-    <row r="27" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="17"/>
-    </row>
-    <row r="28" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="17"/>
-    </row>
-    <row r="29" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="17"/>
-    </row>
-    <row r="30" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="17"/>
-    </row>
-    <row r="31" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="17"/>
-    </row>
-    <row r="32" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="17"/>
-    </row>
-    <row r="33" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="17"/>
-    </row>
-    <row r="34" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="17"/>
-    </row>
-    <row r="35" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="17"/>
-    </row>
-    <row r="36" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="17"/>
-    </row>
-    <row r="37" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="17"/>
-    </row>
-    <row r="38" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="17"/>
-    </row>
-    <row r="39" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="17"/>
-    </row>
-    <row r="40" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="17"/>
-    </row>
-    <row r="41" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="17"/>
-    </row>
-    <row r="42" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="17"/>
-    </row>
-    <row r="43" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="17"/>
-    </row>
-    <row r="44" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="17"/>
-    </row>
-    <row r="45" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="17"/>
-    </row>
-    <row r="46" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="17"/>
-    </row>
-    <row r="47" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="17"/>
-    </row>
-    <row r="48" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="17"/>
-    </row>
-    <row r="49" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="17"/>
-    </row>
-    <row r="50" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="17"/>
-    </row>
-    <row r="51" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="17"/>
-    </row>
-    <row r="52" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="17"/>
-    </row>
-    <row r="53" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="17"/>
-    </row>
-    <row r="54" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="17"/>
-    </row>
-    <row r="55" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="17"/>
-    </row>
-    <row r="56" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="17"/>
-    </row>
-    <row r="57" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="17"/>
-    </row>
-    <row r="58" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="17"/>
-    </row>
-    <row r="59" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="17"/>
-    </row>
-    <row r="60" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="17"/>
-    </row>
-    <row r="61" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="17"/>
-    </row>
-    <row r="62" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="17"/>
-    </row>
-    <row r="63" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="17"/>
-    </row>
-    <row r="64" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="17"/>
-    </row>
-    <row r="65" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="17"/>
-    </row>
-    <row r="66" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="17"/>
-    </row>
-    <row r="67" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="17"/>
-    </row>
-    <row r="68" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="17"/>
-    </row>
-    <row r="69" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="17"/>
-    </row>
-    <row r="70" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="17"/>
-    </row>
-    <row r="71" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="17"/>
-    </row>
-    <row r="72" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="17"/>
-    </row>
-    <row r="73" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="17"/>
-    </row>
-    <row r="74" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="17"/>
-    </row>
-    <row r="75" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="17"/>
-    </row>
-    <row r="76" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="17"/>
-    </row>
-    <row r="77" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="17"/>
-    </row>
-    <row r="78" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="17"/>
-    </row>
-    <row r="79" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="17"/>
-    </row>
-    <row r="80" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="17"/>
-    </row>
-    <row r="81" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="17"/>
-    </row>
-    <row r="82" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="17"/>
-    </row>
-    <row r="83" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="17"/>
-    </row>
-    <row r="84" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="17"/>
-    </row>
-    <row r="85" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="17"/>
-    </row>
-    <row r="86" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="17"/>
-    </row>
-    <row r="87" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="17"/>
-    </row>
-    <row r="88" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="17"/>
-    </row>
-    <row r="89" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="17"/>
-    </row>
-    <row r="90" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="17"/>
-    </row>
-    <row r="91" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="17"/>
-    </row>
-    <row r="92" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="17"/>
-    </row>
-    <row r="93" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="17"/>
-    </row>
-    <row r="94" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="17"/>
-    </row>
-    <row r="95" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="17"/>
-    </row>
-    <row r="96" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="17"/>
-    </row>
-    <row r="97" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="17"/>
-    </row>
-    <row r="98" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="17"/>
-    </row>
-    <row r="99" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="17"/>
-    </row>
-    <row r="100" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="17"/>
-    </row>
-    <row r="101" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="17"/>
-    </row>
-    <row r="102" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="17"/>
-    </row>
-    <row r="103" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="17"/>
-    </row>
-    <row r="104" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="17"/>
-    </row>
-    <row r="105" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="17"/>
-    </row>
-    <row r="106" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="17"/>
-    </row>
-    <row r="107" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="17"/>
-    </row>
-    <row r="108" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="17"/>
-    </row>
-    <row r="109" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="17"/>
-    </row>
-    <row r="110" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="17"/>
-    </row>
-    <row r="111" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="17"/>
-    </row>
-    <row r="112" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="17"/>
-    </row>
-    <row r="113" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="17"/>
-    </row>
-    <row r="114" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="17"/>
-    </row>
-    <row r="115" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="17"/>
-    </row>
-    <row r="116" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="17"/>
-    </row>
-    <row r="117" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="17"/>
-    </row>
-    <row r="118" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="17"/>
-    </row>
-    <row r="119" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="17"/>
-    </row>
-    <row r="120" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="17"/>
-    </row>
-    <row r="121" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="17"/>
-    </row>
-    <row r="122" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="17"/>
-    </row>
-    <row r="123" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="17"/>
-    </row>
-    <row r="124" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="17"/>
-    </row>
-    <row r="125" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="17"/>
-    </row>
-    <row r="126" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="17"/>
-    </row>
-    <row r="127" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="17"/>
-    </row>
-    <row r="128" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="17"/>
-    </row>
-    <row r="129" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="17"/>
-    </row>
-    <row r="130" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="17"/>
-    </row>
-    <row r="131" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="17"/>
-    </row>
-    <row r="132" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="17"/>
-    </row>
-    <row r="133" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="17"/>
-    </row>
-    <row r="134" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="17"/>
-    </row>
-    <row r="135" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="17"/>
-    </row>
-    <row r="136" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="17"/>
-    </row>
-    <row r="137" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="17"/>
-    </row>
-    <row r="138" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="17"/>
-    </row>
-    <row r="139" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="17"/>
-    </row>
-    <row r="140" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="17"/>
-    </row>
-    <row r="141" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="17"/>
-    </row>
-    <row r="142" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="17"/>
-    </row>
-    <row r="143" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="17"/>
-    </row>
-    <row r="144" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="17"/>
-    </row>
-    <row r="145" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="17"/>
-    </row>
-    <row r="146" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="17"/>
-    </row>
-    <row r="147" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="17"/>
-    </row>
-    <row r="148" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="17"/>
-    </row>
-    <row r="149" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A149" s="17"/>
-    </row>
-    <row r="150" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="17"/>
-    </row>
-    <row r="151" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A151" s="17"/>
-    </row>
-    <row r="152" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="17"/>
-    </row>
-    <row r="153" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="17"/>
-    </row>
-    <row r="154" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A154" s="17"/>
-    </row>
-    <row r="155" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A155" s="17"/>
-    </row>
-    <row r="156" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A156" s="17"/>
-    </row>
-    <row r="157" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A157" s="17"/>
-    </row>
-    <row r="158" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A158" s="17"/>
-    </row>
-    <row r="159" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A159" s="17"/>
-    </row>
-    <row r="160" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A160" s="17"/>
-    </row>
-    <row r="161" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A161" s="17"/>
-    </row>
-    <row r="162" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A162" s="17"/>
-    </row>
-    <row r="163" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A163" s="17"/>
-    </row>
-    <row r="164" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A164" s="17"/>
-    </row>
-    <row r="165" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A165" s="17"/>
-    </row>
-    <row r="166" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A166" s="17"/>
-    </row>
-    <row r="167" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A167" s="17"/>
-    </row>
-    <row r="168" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A168" s="17"/>
-    </row>
-    <row r="169" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A169" s="17"/>
-    </row>
-    <row r="170" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A170" s="17"/>
-    </row>
-    <row r="171" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A171" s="17"/>
-    </row>
-    <row r="172" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A172" s="17"/>
-    </row>
-    <row r="173" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A173" s="17"/>
-    </row>
-    <row r="174" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A174" s="17"/>
-    </row>
-    <row r="175" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A175" s="17"/>
-    </row>
-    <row r="176" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A176" s="17"/>
-    </row>
-    <row r="177" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A177" s="17"/>
-    </row>
-    <row r="178" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A178" s="17"/>
-    </row>
-    <row r="179" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A179" s="17"/>
-    </row>
-    <row r="180" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A180" s="17"/>
-    </row>
-    <row r="181" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A181" s="17"/>
-    </row>
-    <row r="182" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A182" s="17"/>
-    </row>
-    <row r="183" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A183" s="17"/>
-    </row>
-    <row r="184" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A184" s="17"/>
-    </row>
-    <row r="185" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A185" s="17"/>
-    </row>
-    <row r="186" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A186" s="17"/>
-    </row>
-    <row r="187" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A187" s="17"/>
-    </row>
-    <row r="188" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A188" s="17"/>
-    </row>
-    <row r="189" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A189" s="17"/>
-    </row>
-    <row r="190" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A190" s="17"/>
-    </row>
-    <row r="191" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A191" s="17"/>
-    </row>
-    <row r="192" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A192" s="17"/>
-    </row>
-    <row r="193" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A193" s="17"/>
-    </row>
-    <row r="194" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A194" s="17"/>
-    </row>
-    <row r="195" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A195" s="17"/>
-    </row>
-    <row r="196" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A196" s="17"/>
-    </row>
-    <row r="197" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A197" s="17"/>
-    </row>
-    <row r="198" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A198" s="17"/>
-    </row>
-    <row r="199" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A199" s="17"/>
-    </row>
-    <row r="200" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A200" s="17"/>
-    </row>
-    <row r="201" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A201" s="17"/>
-    </row>
-    <row r="202" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A202" s="17"/>
-    </row>
-    <row r="203" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A203" s="17"/>
-    </row>
-    <row r="204" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A204" s="17"/>
-    </row>
-    <row r="205" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A205" s="17"/>
-    </row>
-    <row r="206" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A206" s="17"/>
-    </row>
-    <row r="207" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A207" s="17"/>
-    </row>
-    <row r="208" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A208" s="17"/>
-    </row>
-    <row r="209" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A209" s="17"/>
-    </row>
-    <row r="210" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A210" s="17"/>
-    </row>
-    <row r="211" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A211" s="17"/>
-    </row>
-    <row r="212" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A212" s="17"/>
-    </row>
-    <row r="213" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A213" s="17"/>
-    </row>
-    <row r="214" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A214" s="17"/>
-    </row>
-    <row r="215" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A215" s="17"/>
-    </row>
-    <row r="216" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A216" s="17"/>
-    </row>
-    <row r="217" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A217" s="17"/>
-    </row>
-    <row r="218" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A218" s="17"/>
-    </row>
-    <row r="219" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A219" s="17"/>
-    </row>
-    <row r="220" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A220" s="17"/>
-    </row>
-    <row r="221" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A221" s="17"/>
-    </row>
-    <row r="222" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A222" s="17"/>
-    </row>
-    <row r="223" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A223" s="17"/>
-    </row>
-    <row r="224" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A224" s="17"/>
-    </row>
-    <row r="225" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A225" s="17"/>
-    </row>
-    <row r="226" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A226" s="17"/>
-    </row>
-    <row r="227" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A227" s="17"/>
-    </row>
-    <row r="228" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A228" s="17"/>
-    </row>
-    <row r="229" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A229" s="17"/>
-    </row>
-    <row r="230" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A230" s="17"/>
-    </row>
-    <row r="231" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A231" s="17"/>
-    </row>
-    <row r="232" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A232" s="17"/>
-    </row>
-    <row r="233" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A233" s="17"/>
-    </row>
-    <row r="234" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A234" s="17"/>
-    </row>
-    <row r="235" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A235" s="17"/>
-    </row>
-    <row r="236" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A236" s="17"/>
-    </row>
-    <row r="237" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A237" s="17"/>
-    </row>
-    <row r="238" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A238" s="17"/>
-    </row>
-    <row r="239" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A239" s="17"/>
-    </row>
-    <row r="240" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A240" s="17"/>
-    </row>
-    <row r="241" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A241" s="17"/>
-    </row>
-    <row r="242" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A242" s="17"/>
-    </row>
-    <row r="243" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A243" s="17"/>
-    </row>
-    <row r="244" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A244" s="17"/>
-    </row>
-    <row r="245" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A245" s="17"/>
-    </row>
-    <row r="246" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A246" s="17"/>
-    </row>
-    <row r="247" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A247" s="17"/>
-    </row>
-    <row r="248" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A248" s="17"/>
-    </row>
-    <row r="249" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A249" s="17"/>
-    </row>
-    <row r="250" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A250" s="17"/>
-    </row>
-    <row r="251" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A251" s="17"/>
-    </row>
-    <row r="252" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A252" s="17"/>
-    </row>
-    <row r="253" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A253" s="17"/>
-    </row>
-    <row r="254" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A254" s="17"/>
-    </row>
-    <row r="255" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A255" s="17"/>
-    </row>
-    <row r="256" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A256" s="17"/>
-    </row>
-    <row r="257" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A257" s="17"/>
-    </row>
-    <row r="258" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A258" s="17"/>
-    </row>
-    <row r="259" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A259" s="17"/>
-    </row>
-    <row r="260" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A260" s="17"/>
-    </row>
-    <row r="261" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A261" s="17"/>
-    </row>
-    <row r="262" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A262" s="17"/>
-    </row>
-    <row r="263" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A263" s="17"/>
-    </row>
-    <row r="264" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A264" s="17"/>
-    </row>
-    <row r="265" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A265" s="17"/>
-    </row>
-    <row r="266" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A266" s="17"/>
-    </row>
-    <row r="267" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A267" s="17"/>
-    </row>
-    <row r="268" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A268" s="17"/>
-    </row>
-    <row r="269" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A269" s="17"/>
-    </row>
-    <row r="270" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A270" s="17"/>
-    </row>
-    <row r="271" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A271" s="17"/>
-    </row>
-    <row r="272" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A272" s="17"/>
-    </row>
-    <row r="273" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A273" s="17"/>
-    </row>
-    <row r="274" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A274" s="17"/>
-    </row>
-    <row r="275" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A275" s="17"/>
-    </row>
-    <row r="276" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A276" s="17"/>
-    </row>
-    <row r="277" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A277" s="17"/>
-    </row>
-    <row r="278" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A278" s="17"/>
-    </row>
-    <row r="279" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A279" s="17"/>
-    </row>
-    <row r="280" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A280" s="17"/>
-    </row>
-    <row r="281" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A281" s="17"/>
-    </row>
-    <row r="282" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A282" s="17"/>
-    </row>
-    <row r="283" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A283" s="17"/>
-    </row>
-    <row r="284" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A284" s="17"/>
-    </row>
-    <row r="285" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A285" s="17"/>
-    </row>
-    <row r="286" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A286" s="17"/>
-    </row>
-    <row r="287" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A287" s="17"/>
-    </row>
-    <row r="288" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A288" s="17"/>
-    </row>
-    <row r="289" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A289" s="17"/>
-    </row>
-    <row r="290" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A290" s="17"/>
-    </row>
-    <row r="291" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A291" s="17"/>
-    </row>
-    <row r="292" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A292" s="17"/>
-    </row>
-    <row r="293" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A293" s="17"/>
-    </row>
-    <row r="294" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A294" s="17"/>
-    </row>
-    <row r="295" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A295" s="17"/>
-    </row>
-    <row r="296" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A296" s="17"/>
-    </row>
-    <row r="297" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A297" s="17"/>
-    </row>
-    <row r="298" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A298" s="17"/>
-    </row>
-    <row r="299" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A299" s="17"/>
-    </row>
-    <row r="300" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A300" s="17"/>
-    </row>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
+      <c r="P2" s="17"/>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="17"/>
+    </row>
+    <row r="3" spans="3:18" ht="75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="3:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="3:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="3:18" s="7" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="3:18" s="7" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="3:18" s="7" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="3:18" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="3:18" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="3:18" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="3:18" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="3:18" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="3:18" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="3:18" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="3:18" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="17" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="18" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="21" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="22" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="24" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="55" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="56" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="57" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="58" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="59" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="60" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="61" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="62" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="63" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="64" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="65" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="66" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="67" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="68" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="69" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="70" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="71" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="72" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="73" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="74" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="75" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="76" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="77" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="78" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="79" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="80" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="81" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="82" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="83" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="84" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="85" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="86" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="87" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="88" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="89" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="90" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="91" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="92" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="93" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="94" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="95" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="96" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="97" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="98" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="99" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="100" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="101" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="102" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="103" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="104" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="105" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="106" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="107" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="108" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="109" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="110" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="111" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="112" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="113" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="114" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="115" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="116" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="117" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="118" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="119" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="120" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="121" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="122" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="123" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="124" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="125" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="126" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="127" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="128" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="129" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="130" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="131" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="132" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="133" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="134" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="135" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="136" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="137" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="138" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="139" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="140" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="141" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="142" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="143" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="144" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="145" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="146" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="147" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="148" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="149" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="150" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="151" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="152" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="153" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="154" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="155" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="156" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="157" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="158" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="159" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="160" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="161" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="162" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="163" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="164" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="165" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="166" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="167" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="168" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="169" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="170" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="171" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="172" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="173" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="174" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="175" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="176" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="177" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="178" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="179" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="180" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="181" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="182" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="183" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="184" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="185" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="186" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="187" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="188" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="189" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="190" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="191" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="192" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="193" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="194" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="195" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="196" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="197" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="198" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="199" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="200" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="201" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="202" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="203" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="204" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="205" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="206" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="207" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="208" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="209" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="210" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="211" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="212" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="213" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="214" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="215" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="216" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="217" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="218" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="219" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="220" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="221" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="222" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="223" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="224" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="225" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="226" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="227" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="228" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="229" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="230" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="231" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="232" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="233" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="234" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="235" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="236" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="237" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="238" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="239" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="240" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="241" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="242" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="243" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="244" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="245" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="246" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="247" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="248" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="249" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="250" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="251" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="252" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="253" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="254" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="255" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="256" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="257" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="258" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="259" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="260" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="261" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="262" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="263" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="264" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="265" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="266" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="267" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="268" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="269" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="270" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="271" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="272" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="273" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="274" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="275" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="276" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="277" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="278" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="279" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="280" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="281" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="282" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="283" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="284" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="285" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="286" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="287" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="288" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="289" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="290" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="291" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="292" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="293" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="294" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="295" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="296" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="297" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="298" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="299" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="300" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
@@ -26745,6 +26157,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="851b35d3-0456-4d6a-bc2f-da927e91d158">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="19483571-f922-4e8e-9c1c-26f0a2252132" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010001E48B58A68BE64E9120D347E3E06B3A" ma:contentTypeVersion="19" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="2f90046ec77328b7f86417d2e03b3d33">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="851b35d3-0456-4d6a-bc2f-da927e91d158" xmlns:ns3="19483571-f922-4e8e-9c1c-26f0a2252132" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c815006ac2d4f05ee97fdd57e40d8e38" ns2:_="" ns3:_="">
     <xsd:import namespace="851b35d3-0456-4d6a-bc2f-da927e91d158"/>
@@ -26999,27 +26431,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FFD3D529-BCD3-4ECD-9B2A-42924892FFCB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="851b35d3-0456-4d6a-bc2f-da927e91d158"/>
+    <ds:schemaRef ds:uri="19483571-f922-4e8e-9c1c-26f0a2252132"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="851b35d3-0456-4d6a-bc2f-da927e91d158">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="19483571-f922-4e8e-9c1c-26f0a2252132" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3B4D9D5-B351-46EB-A728-C3362FE437D4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{32608D25-EC36-42FE-A1DC-F778995A6799}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -27036,23 +26467,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3B4D9D5-B351-46EB-A728-C3362FE437D4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FFD3D529-BCD3-4ECD-9B2A-42924892FFCB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="851b35d3-0456-4d6a-bc2f-da927e91d158"/>
-    <ds:schemaRef ds:uri="19483571-f922-4e8e-9c1c-26f0a2252132"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>